<commit_message>
first bash at some agGrid changes - lots more to do but getting there. mainly changed excel and a few dates
</commit_message>
<xml_diff>
--- a/DataSets/PriceBlotterCDSIndex.xlsx
+++ b/DataSets/PriceBlotterCDSIndex.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Source\Repos\adaptableblotter-demo\DataSets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdaptableTools/adaptableblotter-demo/DataSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31095" windowHeight="15045"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31100" windowHeight="15040"/>
   </bookViews>
   <sheets>
     <sheet name="CDSIndexPrice" sheetId="3" r:id="rId1"/>
     <sheet name="CdsIndices" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1407,7 +1410,7 @@
     <t>Spread10Y</t>
   </si>
   <si>
-    <t>updated</t>
+    <t>Updated Date</t>
   </si>
 </sst>
 </file>
@@ -2239,20 +2242,20 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>447</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>19257.322228430399</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>3357.2760093665397</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2386,7 +2389,7 @@
         <v>3893.2974723849302</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>7937.8313177125201</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>7644.30655837208</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>8073.2337492083288</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>8966.9483942607203</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>9559.1827792198292</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>10026.6775099309</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>10695.6033565501</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>11242.4350131678</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>10504.423964823798</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2746,7 +2749,7 @@
         <v>10548.3887500574</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2791,7 +2794,7 @@
         <v>10674.582225699</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>11029.918561054001</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>11043.0487013984</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>11312.732254324001</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3007,7 +3010,7 @@
         <v>11882.7810987496</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3061,7 +3064,7 @@
         <v>12221.81170686</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3115,7 +3118,7 @@
         <v>12024.427684104499</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3169,7 +3172,7 @@
         <v>11615.8495524187</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -3196,7 +3199,7 @@
         <v>16762.176684112899</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>16352.083006237897</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -3250,7 +3253,7 @@
         <v>17169.159980757202</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>15133.715498387999</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>14596.6815883772</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -3331,7 +3334,7 @@
         <v>15318.000343827</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>15770.5204417062</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -3385,7 +3388,7 @@
         <v>16608.422765010102</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3412,7 +3415,7 @@
         <v>17201.2942845035</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3439,7 +3442,7 @@
         <v>18003.898135358897</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>19375.103737605699</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -3511,7 +3514,7 @@
         <v>19721.883159208603</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>19520.180242482002</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>17828.941286516998</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -3619,7 +3622,7 @@
         <v>18233.382329358701</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -3655,7 +3658,7 @@
         <v>18530.041354994497</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -3691,7 +3694,7 @@
         <v>19710.839247129599</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -3727,7 +3730,7 @@
         <v>23595.781246696803</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -3763,7 +3766,7 @@
         <v>23063.298962914898</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>23484.013417330298</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -3835,7 +3838,7 @@
         <v>23629.506509741303</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>5162.9487434540897</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -3889,7 +3892,7 @@
         <v>32839.270998436805</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -3916,7 +3919,7 @@
         <v>22280.446250236397</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -3943,7 +3946,7 @@
         <v>9429.7803653687879</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -3970,7 +3973,7 @@
         <v>10399.1866825413</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -3997,7 +4000,7 @@
         <v>10239.524342385001</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -4033,7 +4036,7 @@
         <v>11254.743616956501</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>11655.220461253601</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -4105,7 +4108,7 @@
         <v>12746.2430969094</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -4141,7 +4144,7 @@
         <v>16666.564153215499</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>18351.0735507809</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -4231,7 +4234,7 @@
         <v>23392.6975129858</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -4276,7 +4279,7 @@
         <v>24124.069911757098</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>25179.490579065303</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -4375,7 +4378,7 @@
         <v>26521.784043093299</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -4429,7 +4432,7 @@
         <v>26152.342395283496</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -4483,7 +4486,7 @@
         <v>29142.7581174365</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -4537,7 +4540,7 @@
         <v>39605.046638379201</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -4591,7 +4594,7 @@
         <v>39213.639350885896</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -4645,7 +4648,7 @@
         <v>40798.601403784196</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -4721,21 +4724,21 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>447</v>
       </c>
@@ -4767,7 +4770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4799,7 +4802,7 @@
         <v>1.92573222284304E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -4831,7 +4834,7 @@
         <v>1.92573222284304E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4863,7 +4866,7 @@
         <v>3.3572760093665398E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -4895,7 +4898,7 @@
         <v>3.3572760093665398E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4927,7 +4930,7 @@
         <v>3.8932974723849302E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -4959,7 +4962,7 @@
         <v>3.8932974723849302E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4991,7 +4994,7 @@
         <v>7.9378313177125206E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5023,7 +5026,7 @@
         <v>7.6443065583720804E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -5055,7 +5058,7 @@
         <v>8.0732337492083299E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5087,7 +5090,7 @@
         <v>8.9669483942607202E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>1.8575812070809002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -5151,7 +5154,7 @@
         <v>9.5591827792198304E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -5183,7 +5186,7 @@
         <v>1.15231796524594E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -5215,7 +5218,7 @@
         <v>1.0026677509930901E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -5247,7 +5250,7 @@
         <v>8.6637215685837193E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -5279,7 +5282,7 @@
         <v>1.06956033565501E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -5311,7 +5314,7 @@
         <v>8.2665276660324992E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v>1.12424350131678E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -5375,7 +5378,7 @@
         <v>1.8354451143667499E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -5407,7 +5410,7 @@
         <v>7.9436362364501203E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -5439,7 +5442,7 @@
         <v>1.05044239648238E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -5471,7 +5474,7 @@
         <v>2.9412638892014E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -5503,7 +5506,7 @@
         <v>6.0822062478195901E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -5535,7 +5538,7 @@
         <v>1.05483887500574E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -5567,7 +5570,7 @@
         <v>3.3479033836787101E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -5599,7 +5602,7 @@
         <v>6.3256273300072701E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -5631,7 +5634,7 @@
         <v>1.0674582225699E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -5663,7 +5666,7 @@
         <v>3.9662655812541404E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -5695,7 +5698,7 @@
         <v>6.8580123925151499E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -5727,7 +5730,7 @@
         <v>1.1029918561054E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -5759,7 +5762,7 @@
         <v>2.38716470044086E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -5791,7 +5794,7 @@
         <v>4.4713408982800899E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -5823,7 +5826,7 @@
         <v>7.5006179255964001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -5855,7 +5858,7 @@
         <v>1.1043048701398399E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v>2.3008679783216301E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -5919,7 +5922,7 @@
         <v>5.1646192461741701E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -5951,7 +5954,7 @@
         <v>8.0742284983667603E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -5983,7 +5986,7 @@
         <v>1.1312732254324E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -6015,7 +6018,7 @@
         <v>2.8506258795824701E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -6047,7 +6050,7 @@
         <v>5.72316220291151E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -6079,7 +6082,7 @@
         <v>8.7157416118066808E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -6111,7 +6114,7 @@
         <v>1.1882781098749601E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -6143,7 +6146,7 @@
         <v>3.9613422155401496E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -6175,7 +6178,7 @@
         <v>6.8268314239689296E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -6207,7 +6210,7 @@
         <v>9.6739497290443104E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -6239,7 +6242,7 @@
         <v>1.222181170686E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -6271,7 +6274,7 @@
         <v>4.5758539628816897E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -6303,7 +6306,7 @@
         <v>7.6117267090422703E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -6335,7 +6338,7 @@
         <v>1.0362332080842199E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -6367,7 +6370,7 @@
         <v>1.2024427684104499E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -6399,7 +6402,7 @@
         <v>5.2784380822277002E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -6431,7 +6434,7 @@
         <v>8.1795991320831804E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -6463,7 +6466,7 @@
         <v>1.04787979282708E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -6495,7 +6498,7 @@
         <v>1.16158495524187E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -6527,7 +6530,7 @@
         <v>5.3382030293634497E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -6559,7 +6562,7 @@
         <v>8.2169150200523001E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -6591,7 +6594,7 @@
         <v>1.02488358455914E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -6623,7 +6626,7 @@
         <v>1.6762176684112898E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -6655,7 +6658,7 @@
         <v>1.6352083006237899E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -6687,7 +6690,7 @@
         <v>1.7169159980757201E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -6719,7 +6722,7 @@
         <v>1.5133715498388E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -6751,7 +6754,7 @@
         <v>1.45966815883772E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -6783,7 +6786,7 @@
         <v>1.5318000343827E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -6815,7 +6818,7 @@
         <v>1.5770520441706199E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -6847,7 +6850,7 @@
         <v>1.6608422765010102E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -6879,7 +6882,7 @@
         <v>1.72012942845035E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -6911,7 +6914,7 @@
         <v>1.8003898135358899E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -6943,7 +6946,7 @@
         <v>1.93751037376057E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -6975,7 +6978,7 @@
         <v>1.3592890803289501E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -7007,7 +7010,7 @@
         <v>1.97218831592086E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -7039,7 +7042,7 @@
         <v>1.3457416164892801E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -7071,7 +7074,7 @@
         <v>1.9520180242482001E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -7103,7 +7106,7 @@
         <v>1.3788192340587899E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -7135,7 +7138,7 @@
         <v>1.7828941286516999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -7167,7 +7170,7 @@
         <v>1.0936923607378799E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -7199,7 +7202,7 @@
         <v>1.8233382329358699E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -7231,7 +7234,7 @@
         <v>1.15059615771387E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>1.85300413549945E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -7295,7 +7298,7 @@
         <v>1.24383366258868E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -7327,7 +7330,7 @@
         <v>1.9710839247129599E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -7359,7 +7362,7 @@
         <v>1.3531243474431199E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -7391,7 +7394,7 @@
         <v>2.3595781246696802E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -7423,7 +7426,7 @@
         <v>1.7746969433875801E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -7455,7 +7458,7 @@
         <v>2.30632989629149E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -7487,7 +7490,7 @@
         <v>1.8024055481121001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -7519,7 +7522,7 @@
         <v>2.34840134173303E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -7551,7 +7554,7 @@
         <v>1.9275120404733E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -7583,7 +7586,7 @@
         <v>2.3629506509741299E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -7615,7 +7618,7 @@
         <v>2.0141825571130499E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -7647,7 +7650,7 @@
         <v>5.1629799293405002E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -7679,7 +7682,7 @@
         <v>5.16318792893303E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>13</v>
       </c>
@@ -7711,7 +7714,7 @@
         <v>5.1631567465225004E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>13</v>
       </c>
@@ -7743,7 +7746,7 @@
         <v>5.1631567465225004E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>13</v>
       </c>
@@ -7775,7 +7778,7 @@
         <v>5.1629487434540896E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -7807,7 +7810,7 @@
         <v>5.1629487434540896E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -7839,7 +7842,7 @@
         <v>3.2839303925237602E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -7871,7 +7874,7 @@
         <v>3.2839303925237602E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -7903,7 +7906,7 @@
         <v>3.2839270998436802E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -7935,7 +7938,7 @@
         <v>3.2839270998436802E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -7967,7 +7970,7 @@
         <v>3.2839270998436802E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -7999,7 +8002,7 @@
         <v>3.2839270998436802E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>13</v>
       </c>
@@ -8031,7 +8034,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>13</v>
       </c>
@@ -8063,7 +8066,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>13</v>
       </c>
@@ -8095,7 +8098,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -8127,7 +8130,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -8159,7 +8162,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>13</v>
       </c>
@@ -8191,7 +8194,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>13</v>
       </c>
@@ -8223,7 +8226,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -8255,7 +8258,7 @@
         <v>2.2239691821851499E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>13</v>
       </c>
@@ -8287,7 +8290,7 @@
         <v>2.22804462502364E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>13</v>
       </c>
@@ -8319,7 +8322,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -8351,7 +8354,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -8383,7 +8386,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -8415,7 +8418,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -8447,7 +8450,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -8479,7 +8482,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -8511,7 +8514,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>13</v>
       </c>
@@ -8543,7 +8546,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -8575,7 +8578,7 @@
         <v>9.4233111467820693E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -8607,7 +8610,7 @@
         <v>9.4297803653687895E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -8639,7 +8642,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>13</v>
       </c>
@@ -8671,7 +8674,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -8703,7 +8706,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -8735,7 +8738,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>13</v>
       </c>
@@ -8767,7 +8770,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -8799,7 +8802,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -8831,7 +8834,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>13</v>
       </c>
@@ -8863,7 +8866,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -8895,7 +8898,7 @@
         <v>1.0410332636543E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>13</v>
       </c>
@@ -8927,7 +8930,7 @@
         <v>1.0399186682541301E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>13</v>
       </c>
@@ -8959,7 +8962,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>13</v>
       </c>
@@ -8991,7 +8994,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>13</v>
       </c>
@@ -9023,7 +9026,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>13</v>
       </c>
@@ -9055,7 +9058,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -9087,7 +9090,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>13</v>
       </c>
@@ -9119,7 +9122,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>13</v>
       </c>
@@ -9151,7 +9154,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -9183,7 +9186,7 @@
         <v>1.0254444548904101E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -9215,7 +9218,7 @@
         <v>1.0239524342385E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -9247,7 +9250,7 @@
         <v>1.1254743616956501E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -9279,7 +9282,7 @@
         <v>1.1254743616956501E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -9311,7 +9314,7 @@
         <v>1.1254743616956501E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -9343,7 +9346,7 @@
         <v>1.1254743616956501E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>13</v>
       </c>
@@ -9375,7 +9378,7 @@
         <v>1.1254743616956501E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>13</v>
       </c>
@@ -9407,7 +9410,7 @@
         <v>1.1254743616956501E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>13</v>
       </c>
@@ -9439,7 +9442,7 @@
         <v>4.7635605439084001E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>13</v>
       </c>
@@ -9471,7 +9474,7 @@
         <v>4.7635605439084001E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>13</v>
       </c>
@@ -9503,7 +9506,7 @@
         <v>4.7635605439084001E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>13</v>
       </c>
@@ -9535,7 +9538,7 @@
         <v>4.7635605439084001E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>13</v>
       </c>
@@ -9567,7 +9570,7 @@
         <v>4.7635605439084001E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>13</v>
       </c>
@@ -9599,7 +9602,7 @@
         <v>4.7635605439084001E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>13</v>
       </c>
@@ -9631,7 +9634,7 @@
         <v>1.16735844864165E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>13</v>
       </c>
@@ -9663,7 +9666,7 @@
         <v>1.16735844864165E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>13</v>
       </c>
@@ -9695,7 +9698,7 @@
         <v>1.16735844864165E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>13</v>
       </c>
@@ -9727,7 +9730,7 @@
         <v>1.16735844864165E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>13</v>
       </c>
@@ -9759,7 +9762,7 @@
         <v>1.16735844864165E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>13</v>
       </c>
@@ -9791,7 +9794,7 @@
         <v>1.16552204612536E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>13</v>
       </c>
@@ -9823,7 +9826,7 @@
         <v>4.4004651933634304E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>13</v>
       </c>
@@ -9855,7 +9858,7 @@
         <v>4.4004651933634304E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>13</v>
       </c>
@@ -9887,7 +9890,7 @@
         <v>4.4004651933634304E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>13</v>
       </c>
@@ -9919,7 +9922,7 @@
         <v>4.4004651933634304E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>13</v>
       </c>
@@ -9951,7 +9954,7 @@
         <v>4.4004651933634304E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>13</v>
       </c>
@@ -9983,7 +9986,7 @@
         <v>4.4447043154008702E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>13</v>
       </c>
@@ -10015,7 +10018,7 @@
         <v>1.27662001846044E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>13</v>
       </c>
@@ -10047,7 +10050,7 @@
         <v>1.27662001846044E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>13</v>
       </c>
@@ -10079,7 +10082,7 @@
         <v>1.27662001846044E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>13</v>
       </c>
@@ -10111,7 +10114,7 @@
         <v>1.27662001846044E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>13</v>
       </c>
@@ -10143,7 +10146,7 @@
         <v>1.27662001846044E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>13</v>
       </c>
@@ -10175,7 +10178,7 @@
         <v>1.27462430969094E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>13</v>
       </c>
@@ -10207,7 +10210,7 @@
         <v>5.4342438020974996E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>13</v>
       </c>
@@ -10239,7 +10242,7 @@
         <v>5.4342438020974996E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>13</v>
       </c>
@@ -10271,7 +10274,7 @@
         <v>5.4342438020974996E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>13</v>
       </c>
@@ -10303,7 +10306,7 @@
         <v>5.4342438020974996E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>13</v>
       </c>
@@ -10335,7 +10338,7 @@
         <v>5.4342438020974996E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>13</v>
       </c>
@@ -10367,7 +10370,7 @@
         <v>5.4709872003982198E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>13</v>
       </c>
@@ -10399,7 +10402,7 @@
         <v>1.6687574218817901E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>13</v>
       </c>
@@ -10431,7 +10434,7 @@
         <v>1.6687574218817901E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>13</v>
       </c>
@@ -10463,7 +10466,7 @@
         <v>1.6687574218817901E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>13</v>
       </c>
@@ -10495,7 +10498,7 @@
         <v>1.6687574218817901E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>13</v>
       </c>
@@ -10527,7 +10530,7 @@
         <v>1.6666564153215501E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>13</v>
       </c>
@@ -10559,7 +10562,7 @@
         <v>9.3348104279471801E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>13</v>
       </c>
@@ -10591,7 +10594,7 @@
         <v>9.3348104279471801E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>13</v>
       </c>
@@ -10623,7 +10626,7 @@
         <v>9.3348104279471801E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>13</v>
       </c>
@@ -10655,7 +10658,7 @@
         <v>9.3348104279471801E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>13</v>
       </c>
@@ -10687,7 +10690,7 @@
         <v>9.3406346004401807E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>13</v>
       </c>
@@ -10719,7 +10722,7 @@
         <v>1.83761472622214E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>13</v>
       </c>
@@ -10751,7 +10754,7 @@
         <v>1.8378019074837399E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>13</v>
       </c>
@@ -10783,7 +10786,7 @@
         <v>1.8351073550780899E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>13</v>
       </c>
@@ -10815,7 +10818,7 @@
         <v>5.6948119288556497E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>13</v>
       </c>
@@ -10847,7 +10850,7 @@
         <v>5.7182140849699999E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>13</v>
       </c>
@@ -10879,7 +10882,7 @@
         <v>5.7709706702955303E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>13</v>
       </c>
@@ -10911,7 +10914,7 @@
         <v>1.05888558392016E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>13</v>
       </c>
@@ -10943,7 +10946,7 @@
         <v>1.05934986675021E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>13</v>
       </c>
@@ -10975,7 +10978,7 @@
         <v>1.0580973294879399E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>13</v>
       </c>
@@ -11007,7 +11010,7 @@
         <v>2.33926975129858E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>13</v>
       </c>
@@ -11039,7 +11042,7 @@
         <v>2.33926975129858E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>13</v>
       </c>
@@ -11071,7 +11074,7 @@
         <v>2.33926975129858E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>13</v>
       </c>
@@ -11103,7 +11106,7 @@
         <v>2.8551658240970099E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>13</v>
       </c>
@@ -11135,7 +11138,7 @@
         <v>2.8551658240970099E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>13</v>
       </c>
@@ -11167,7 +11170,7 @@
         <v>2.8551658240970099E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>13</v>
       </c>
@@ -11199,7 +11202,7 @@
         <v>1.9206548458349602E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>13</v>
       </c>
@@ -11231,7 +11234,7 @@
         <v>1.9206548458349602E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>13</v>
       </c>
@@ -11263,7 +11266,7 @@
         <v>1.9206548458349602E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>13</v>
       </c>
@@ -11295,7 +11298,7 @@
         <v>2.4124069911757098E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>13</v>
       </c>
@@ -11327,7 +11330,7 @@
         <v>2.4124069911757098E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>13</v>
       </c>
@@ -11359,7 +11362,7 @@
         <v>2.4124069911757098E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>13</v>
       </c>
@@ -11391,7 +11394,7 @@
         <v>2.01367438924995E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>13</v>
       </c>
@@ -11423,7 +11426,7 @@
         <v>2.01367438924995E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>13</v>
       </c>
@@ -11455,7 +11458,7 @@
         <v>2.01367438924995E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>13</v>
       </c>
@@ -11487,7 +11490,7 @@
         <v>1.9100388705320701E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>13</v>
       </c>
@@ -11519,7 +11522,7 @@
         <v>1.9100388705320701E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>13</v>
       </c>
@@ -11551,7 +11554,7 @@
         <v>1.9100388705320701E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>13</v>
       </c>
@@ -11583,7 +11586,7 @@
         <v>2.5179490579065301E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>13</v>
       </c>
@@ -11615,7 +11618,7 @@
         <v>2.5179490579065301E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>13</v>
       </c>
@@ -11647,7 +11650,7 @@
         <v>2.5179490579065301E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>13</v>
       </c>
@@ -11679,7 +11682,7 @@
         <v>1.8800390102747599E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>13</v>
       </c>
@@ -11711,7 +11714,7 @@
         <v>1.8800390102747599E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>13</v>
       </c>
@@ -11743,7 +11746,7 @@
         <v>1.8800390102747599E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>13</v>
       </c>
@@ -11775,7 +11778,7 @@
         <v>2.03153278306623E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>13</v>
       </c>
@@ -11807,7 +11810,7 @@
         <v>2.03153278306623E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>13</v>
       </c>
@@ -11839,7 +11842,7 @@
         <v>2.03153278306623E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>13</v>
       </c>
@@ -11871,7 +11874,7 @@
         <v>2.6521784043093299E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>13</v>
       </c>
@@ -11903,7 +11906,7 @@
         <v>2.6521784043093299E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>13</v>
       </c>
@@ -11935,7 +11938,7 @@
         <v>2.6521784043093299E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>13</v>
       </c>
@@ -11967,7 +11970,7 @@
         <v>4.6311081153606701E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>13</v>
       </c>
@@ -11999,7 +12002,7 @@
         <v>4.6311081153606701E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>13</v>
       </c>
@@ -12031,7 +12034,7 @@
         <v>4.6311081153606701E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>13</v>
       </c>
@@ -12063,7 +12066,7 @@
         <v>1.8439889666227501E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>13</v>
       </c>
@@ -12095,7 +12098,7 @@
         <v>1.8439889666227501E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>13</v>
       </c>
@@ -12127,7 +12130,7 @@
         <v>1.8439889666227501E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>13</v>
       </c>
@@ -12159,7 +12162,7 @@
         <v>2.1629221291661501E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>13</v>
       </c>
@@ -12191,7 +12194,7 @@
         <v>2.1629221291661501E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>13</v>
       </c>
@@ -12223,7 +12226,7 @@
         <v>2.1629221291661501E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>13</v>
       </c>
@@ -12255,7 +12258,7 @@
         <v>2.6152342395283499E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>13</v>
       </c>
@@ -12287,7 +12290,7 @@
         <v>2.6152342395283499E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>13</v>
       </c>
@@ -12319,7 +12322,7 @@
         <v>2.7213066382189E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>13</v>
       </c>
@@ -12351,7 +12354,7 @@
         <v>2.7213066382189E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>13</v>
       </c>
@@ -12383,7 +12386,7 @@
         <v>1.86643067918634E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>13</v>
       </c>
@@ -12415,7 +12418,7 @@
         <v>1.86643067918634E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>13</v>
       </c>
@@ -12447,7 +12450,7 @@
         <v>2.2135643394115698E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>13</v>
       </c>
@@ -12479,7 +12482,7 @@
         <v>2.2135643394115698E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>13</v>
       </c>
@@ -12511,7 +12514,7 @@
         <v>2.9142758117436499E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>13</v>
       </c>
@@ -12543,7 +12546,7 @@
         <v>2.9142758117436499E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>13</v>
       </c>
@@ -12575,7 +12578,7 @@
         <v>2.9142758117436499E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>13</v>
       </c>
@@ -12607,7 +12610,7 @@
         <v>1.91013444580681E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>13</v>
       </c>
@@ -12639,7 +12642,7 @@
         <v>1.91013444580681E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>13</v>
       </c>
@@ -12671,7 +12674,7 @@
         <v>1.91013444580681E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>13</v>
       </c>
@@ -12703,7 +12706,7 @@
         <v>2.0561585272954999E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>13</v>
       </c>
@@ -12735,7 +12738,7 @@
         <v>2.0561585272954999E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>13</v>
       </c>
@@ -12767,7 +12770,7 @@
         <v>2.0561585272954999E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>13</v>
       </c>
@@ -12799,7 +12802,7 @@
         <v>2.5329595479434398E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>13</v>
       </c>
@@ -12831,7 +12834,7 @@
         <v>2.5329595479434398E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>13</v>
       </c>
@@ -12863,7 +12866,7 @@
         <v>2.5329595479434398E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>13</v>
       </c>
@@ -12895,7 +12898,7 @@
         <v>3.9659404586358103E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>13</v>
       </c>
@@ -12927,7 +12930,7 @@
         <v>3.9605046638379202E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>13</v>
       </c>
@@ -12959,7 +12962,7 @@
         <v>3.9605046638379202E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>13</v>
       </c>
@@ -12991,7 +12994,7 @@
         <v>3.1958482267112502E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>13</v>
       </c>
@@ -13023,7 +13026,7 @@
         <v>3.1477241335471397E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>13</v>
       </c>
@@ -13055,7 +13058,7 @@
         <v>3.1477241335471397E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>13</v>
       </c>
@@ -13087,7 +13090,7 @@
         <v>3.37698220747807E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>13</v>
       </c>
@@ -13119,7 +13122,7 @@
         <v>3.3671394520166202E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>13</v>
       </c>
@@ -13151,7 +13154,7 @@
         <v>3.3671394520166202E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>13</v>
       </c>
@@ -13183,7 +13186,7 @@
         <v>3.7718869842517898E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>13</v>
       </c>
@@ -13215,7 +13218,7 @@
         <v>3.7675516712142101E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>13</v>
       </c>
@@ -13247,7 +13250,7 @@
         <v>3.7675516712142101E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>13</v>
       </c>
@@ -13279,7 +13282,7 @@
         <v>3.9228153500307499E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>13</v>
       </c>
@@ -13311,7 +13314,7 @@
         <v>3.9213639350885898E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>13</v>
       </c>
@@ -13343,7 +13346,7 @@
         <v>3.9213639350885898E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>13</v>
       </c>
@@ -13375,7 +13378,7 @@
         <v>2.9159207696595E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>13</v>
       </c>
@@ -13407,7 +13410,7 @@
         <v>2.9104672430977099E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>13</v>
       </c>
@@ -13439,7 +13442,7 @@
         <v>2.9104672430977099E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>13</v>
       </c>
@@ -13471,7 +13474,7 @@
         <v>3.3593909410263197E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>13</v>
       </c>
@@ -13503,7 +13506,7 @@
         <v>3.3625608887559402E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>13</v>
       </c>
@@ -13535,7 +13538,7 @@
         <v>3.3625608887559402E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>13</v>
       </c>
@@ -13567,7 +13570,7 @@
         <v>3.7589367148340602E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>13</v>
       </c>
@@ -13599,7 +13602,7 @@
         <v>3.7586231495436898E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>13</v>
       </c>
@@ -13631,7 +13634,7 @@
         <v>3.7586231495436898E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>13</v>
       </c>
@@ -13663,7 +13666,7 @@
         <v>4.0798601403784197E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>13</v>
       </c>
@@ -13695,7 +13698,7 @@
         <v>3.10026503690051E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>13</v>
       </c>
@@ -13727,7 +13730,7 @@
         <v>3.6077238364814697E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>13</v>
       </c>
@@ -13759,7 +13762,7 @@
         <v>3.9459153635906602E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>13</v>
       </c>
@@ -13791,7 +13794,7 @@
         <v>3.9074227505774099E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>13</v>
       </c>
@@ -13823,7 +13826,7 @@
         <v>2.5993098648778402E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>13</v>
       </c>
@@ -13855,7 +13858,7 @@
         <v>3.3918175338510298E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
creating checkbox for ag grid bool column
</commit_message>
<xml_diff>
--- a/DataSets/PriceBlotterCDSIndex.xlsx
+++ b/DataSets/PriceBlotterCDSIndex.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31100" windowHeight="15040"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740"/>
   </bookViews>
   <sheets>
     <sheet name="CDSIndexPrice" sheetId="3" r:id="rId1"/>
@@ -1912,10 +1912,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2242,7 +2245,7 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2252,7 +2255,7 @@
     <col min="3" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -2301,7 +2304,7 @@
       <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -2327,7 +2330,7 @@
       <c r="O2" t="s">
         <v>60</v>
       </c>
-      <c r="P2" t="b">
+      <c r="P2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q2">
@@ -2354,7 +2357,7 @@
       <c r="O3" t="s">
         <v>153</v>
       </c>
-      <c r="P3" t="b">
+      <c r="P3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q3">
@@ -2381,7 +2384,7 @@
       <c r="O4" t="s">
         <v>62</v>
       </c>
-      <c r="P4" t="b">
+      <c r="P4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q4">
@@ -2408,7 +2411,7 @@
       <c r="O5" t="s">
         <v>28</v>
       </c>
-      <c r="P5" t="b">
+      <c r="P5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q5">
@@ -2435,7 +2438,7 @@
       <c r="O6" t="s">
         <v>34</v>
       </c>
-      <c r="P6" t="b">
+      <c r="P6" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q6">
@@ -2462,7 +2465,7 @@
       <c r="O7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" t="b">
+      <c r="P7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q7">
@@ -2498,7 +2501,7 @@
       <c r="O8" t="s">
         <v>44</v>
       </c>
-      <c r="P8" t="b">
+      <c r="P8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q8">
@@ -2534,7 +2537,7 @@
       <c r="O9" t="s">
         <v>75</v>
       </c>
-      <c r="P9" t="b">
+      <c r="P9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q9">
@@ -2570,7 +2573,7 @@
       <c r="O10" t="s">
         <v>101</v>
       </c>
-      <c r="P10" t="b">
+      <c r="P10" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q10">
@@ -2606,7 +2609,7 @@
       <c r="O11" t="s">
         <v>136</v>
       </c>
-      <c r="P11" t="b">
+      <c r="P11" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q11">
@@ -2651,7 +2654,7 @@
       <c r="O12" t="s">
         <v>142</v>
       </c>
-      <c r="P12" t="b">
+      <c r="P12" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q12">
@@ -2696,7 +2699,7 @@
       <c r="O13" t="s">
         <v>158</v>
       </c>
-      <c r="P13" t="b">
+      <c r="P13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q13">
@@ -2741,7 +2744,7 @@
       <c r="O14" t="s">
         <v>197</v>
       </c>
-      <c r="P14" t="b">
+      <c r="P14" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q14">
@@ -2786,7 +2789,7 @@
       <c r="O15" t="s">
         <v>235</v>
       </c>
-      <c r="P15" t="b">
+      <c r="P15" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q15">
@@ -2840,7 +2843,7 @@
       <c r="O16" t="s">
         <v>242</v>
       </c>
-      <c r="P16" t="b">
+      <c r="P16" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q16">
@@ -2894,7 +2897,7 @@
       <c r="O17" t="s">
         <v>260</v>
       </c>
-      <c r="P17" t="b">
+      <c r="P17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q17">
@@ -2948,7 +2951,7 @@
       <c r="O18" t="s">
         <v>309</v>
       </c>
-      <c r="P18" t="b">
+      <c r="P18" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q18">
@@ -3002,7 +3005,7 @@
       <c r="O19" t="s">
         <v>322</v>
       </c>
-      <c r="P19" t="b">
+      <c r="P19" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q19">
@@ -3056,7 +3059,7 @@
       <c r="O20" t="s">
         <v>332</v>
       </c>
-      <c r="P20" t="b">
+      <c r="P20" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q20">
@@ -3110,7 +3113,7 @@
       <c r="O21" t="s">
         <v>353</v>
       </c>
-      <c r="P21" t="b">
+      <c r="P21" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q21">
@@ -3164,7 +3167,7 @@
       <c r="O22" t="s">
         <v>373</v>
       </c>
-      <c r="P22" t="b">
+      <c r="P22" s="5" t="b">
         <v>1</v>
       </c>
       <c r="Q22">
@@ -3191,7 +3194,7 @@
       <c r="O23" t="s">
         <v>17</v>
       </c>
-      <c r="P23" t="b">
+      <c r="P23" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q23">
@@ -3218,7 +3221,7 @@
       <c r="O24" t="s">
         <v>22</v>
       </c>
-      <c r="P24" t="b">
+      <c r="P24" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q24">
@@ -3245,7 +3248,7 @@
       <c r="O25" t="s">
         <v>26</v>
       </c>
-      <c r="P25" t="b">
+      <c r="P25" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q25">
@@ -3272,7 +3275,7 @@
       <c r="O26" t="s">
         <v>30</v>
       </c>
-      <c r="P26" t="b">
+      <c r="P26" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q26">
@@ -3299,7 +3302,7 @@
       <c r="O27" t="s">
         <v>52</v>
       </c>
-      <c r="P27" t="b">
+      <c r="P27" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q27">
@@ -3326,7 +3329,7 @@
       <c r="O28" t="s">
         <v>54</v>
       </c>
-      <c r="P28" t="b">
+      <c r="P28" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q28">
@@ -3353,7 +3356,7 @@
       <c r="O29" t="s">
         <v>56</v>
       </c>
-      <c r="P29" t="b">
+      <c r="P29" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q29">
@@ -3380,7 +3383,7 @@
       <c r="O30" t="s">
         <v>71</v>
       </c>
-      <c r="P30" t="b">
+      <c r="P30" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q30">
@@ -3407,7 +3410,7 @@
       <c r="O31" t="s">
         <v>96</v>
       </c>
-      <c r="P31" t="b">
+      <c r="P31" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q31">
@@ -3434,7 +3437,7 @@
       <c r="O32" t="s">
         <v>134</v>
       </c>
-      <c r="P32" t="b">
+      <c r="P32" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q32">
@@ -3470,7 +3473,7 @@
       <c r="O33" t="s">
         <v>146</v>
       </c>
-      <c r="P33" t="b">
+      <c r="P33" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q33">
@@ -3506,7 +3509,7 @@
       <c r="O34" t="s">
         <v>166</v>
       </c>
-      <c r="P34" t="b">
+      <c r="P34" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q34">
@@ -3542,7 +3545,7 @@
       <c r="O35" t="s">
         <v>201</v>
       </c>
-      <c r="P35" t="b">
+      <c r="P35" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q35">
@@ -3578,7 +3581,7 @@
       <c r="O36" t="s">
         <v>228</v>
       </c>
-      <c r="P36" t="b">
+      <c r="P36" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q36">
@@ -3614,7 +3617,7 @@
       <c r="O37" t="s">
         <v>239</v>
       </c>
-      <c r="P37" t="b">
+      <c r="P37" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q37">
@@ -3650,7 +3653,7 @@
       <c r="O38" t="s">
         <v>257</v>
       </c>
-      <c r="P38" t="b">
+      <c r="P38" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q38">
@@ -3686,7 +3689,7 @@
       <c r="O39" t="s">
         <v>306</v>
       </c>
-      <c r="P39" t="b">
+      <c r="P39" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q39">
@@ -3722,7 +3725,7 @@
       <c r="O40" t="s">
         <v>319</v>
       </c>
-      <c r="P40" t="b">
+      <c r="P40" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q40">
@@ -3758,7 +3761,7 @@
       <c r="O41" t="s">
         <v>342</v>
       </c>
-      <c r="P41" t="b">
+      <c r="P41" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q41">
@@ -3794,7 +3797,7 @@
       <c r="O42" t="s">
         <v>350</v>
       </c>
-      <c r="P42" t="b">
+      <c r="P42" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q42">
@@ -3830,7 +3833,7 @@
       <c r="O43" t="s">
         <v>378</v>
       </c>
-      <c r="P43" t="b">
+      <c r="P43" s="5" t="b">
         <v>1</v>
       </c>
       <c r="Q43">
@@ -3857,7 +3860,7 @@
       <c r="O44" t="s">
         <v>226</v>
       </c>
-      <c r="P44" t="b">
+      <c r="P44" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q44">
@@ -3884,7 +3887,7 @@
       <c r="O45" t="s">
         <v>224</v>
       </c>
-      <c r="P45" t="b">
+      <c r="P45" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q45">
@@ -3911,7 +3914,7 @@
       <c r="O46" t="s">
         <v>386</v>
       </c>
-      <c r="P46" t="b">
+      <c r="P46" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q46">
@@ -3938,7 +3941,7 @@
       <c r="O47" t="s">
         <v>388</v>
       </c>
-      <c r="P47" t="b">
+      <c r="P47" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q47">
@@ -3965,7 +3968,7 @@
       <c r="O48" t="s">
         <v>390</v>
       </c>
-      <c r="P48" t="b">
+      <c r="P48" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q48">
@@ -3992,7 +3995,7 @@
       <c r="O49" t="s">
         <v>392</v>
       </c>
-      <c r="P49" t="b">
+      <c r="P49" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q49">
@@ -4028,7 +4031,7 @@
       <c r="O50" t="s">
         <v>394</v>
       </c>
-      <c r="P50" t="b">
+      <c r="P50" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q50">
@@ -4064,7 +4067,7 @@
       <c r="O51" t="s">
         <v>397</v>
       </c>
-      <c r="P51" t="b">
+      <c r="P51" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q51">
@@ -4100,7 +4103,7 @@
       <c r="O52" t="s">
         <v>400</v>
       </c>
-      <c r="P52" t="b">
+      <c r="P52" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q52">
@@ -4136,7 +4139,7 @@
       <c r="O53" t="s">
         <v>403</v>
       </c>
-      <c r="P53" t="b">
+      <c r="P53" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q53">
@@ -4181,7 +4184,7 @@
       <c r="O54" t="s">
         <v>406</v>
       </c>
-      <c r="P54" t="b">
+      <c r="P54" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q54">
@@ -4226,7 +4229,7 @@
       <c r="O55" t="s">
         <v>410</v>
       </c>
-      <c r="P55" t="b">
+      <c r="P55" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q55">
@@ -4271,7 +4274,7 @@
       <c r="O56" t="s">
         <v>414</v>
       </c>
-      <c r="P56" t="b">
+      <c r="P56" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q56">
@@ -4316,7 +4319,7 @@
       <c r="O57" t="s">
         <v>418</v>
       </c>
-      <c r="P57" t="b">
+      <c r="P57" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q57">
@@ -4370,7 +4373,7 @@
       <c r="O58" t="s">
         <v>422</v>
       </c>
-      <c r="P58" t="b">
+      <c r="P58" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q58">
@@ -4424,7 +4427,7 @@
       <c r="O59" t="s">
         <v>427</v>
       </c>
-      <c r="P59" t="b">
+      <c r="P59" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q59">
@@ -4478,7 +4481,7 @@
       <c r="O60" t="s">
         <v>432</v>
       </c>
-      <c r="P60" t="b">
+      <c r="P60" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q60">
@@ -4532,7 +4535,7 @@
       <c r="O61" t="s">
         <v>437</v>
       </c>
-      <c r="P61" t="b">
+      <c r="P61" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q61">
@@ -4586,7 +4589,7 @@
       <c r="O62" t="s">
         <v>442</v>
       </c>
-      <c r="P62" t="b">
+      <c r="P62" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q62">
@@ -4640,7 +4643,7 @@
       <c r="O63" t="s">
         <v>345</v>
       </c>
-      <c r="P63" t="b">
+      <c r="P63" s="5" t="b">
         <v>0</v>
       </c>
       <c r="Q63">
@@ -4694,7 +4697,7 @@
       <c r="O64" t="s">
         <v>381</v>
       </c>
-      <c r="P64" t="b">
+      <c r="P64" s="5" t="b">
         <v>1</v>
       </c>
       <c r="Q64">

</xml_diff>

<commit_message>
more data changes and kendo updates
</commit_message>
<xml_diff>
--- a/DataSets/PriceBlotterCDSIndex.xlsx
+++ b/DataSets/PriceBlotterCDSIndex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdaptableTools/adaptableblotter-demo/DataSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdaptableTools/Code/adaptableblotter-demo/DataSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1410,7 +1410,7 @@
     <t>Spread10Y</t>
   </si>
   <si>
-    <t>Updated Date</t>
+    <t>UpdatedDate</t>
   </si>
 </sst>
 </file>
@@ -2246,7 +2246,7 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>